<commit_message>
Tested functionality of the methods to see if they perform as expected.
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Desktop\Intermediate Software Development0315\8. Activities\Module_01\given_files\activity_1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e96da391a30bed48/Documents/intermediate_software_development/activities/activity_1/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF8B5DF3-4676-4A22-A51D-E7D607652C6E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -249,6 +249,42 @@
   </si>
   <si>
     <t>Attribute  set to input values.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>("DUNE", "Frank Herbert", Genre.FICTION)</t>
+  </si>
+  <si>
+    <t>("", "Frank Herbert", Genre.FICTION)</t>
+  </si>
+  <si>
+    <t>("DUNE", "", Genre.FICTION)</t>
+  </si>
+  <si>
+    <t>("DUNE", "Frank Herbert", "INVALID)</t>
+  </si>
+  <si>
+    <t>Pass/No errors</t>
+  </si>
+  <si>
+    <t>Raise ValueError</t>
+  </si>
+  <si>
+    <t>LibraryItem("DUNE", "Frank Herbert", Genre.FICTION)</t>
+  </si>
+  <si>
+    <t>Returns title</t>
+  </si>
+  <si>
+    <t>Returns author</t>
+  </si>
+  <si>
+    <t>Returns genre</t>
+  </si>
+  <si>
+    <t>Philip Pacla-on</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1146,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1176,9 @@
       <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1186,9 +1224,15 @@
       <c r="D7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1201,9 +1245,15 @@
       <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="E8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -1216,9 +1266,15 @@
       <c r="D9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -1231,9 +1287,15 @@
       <c r="D10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
@@ -1245,9 +1307,15 @@
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
@@ -1259,9 +1327,15 @@
       <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
@@ -1273,9 +1347,15 @@
       <c r="D13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
@@ -1405,9 +1485,10 @@
     <mergeCell ref="B26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new unit testing to item.id & is_borrowed.
</commit_message>
<xml_diff>
--- a/tests/test_plan_library_item.xlsx
+++ b/tests/test_plan_library_item.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e96da391a30bed48/Documents/intermediate_software_development/activities/activity_1/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF8B5DF3-4676-4A22-A51D-E7D607652C6E}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{94801D8B-F184-4C7C-AC17-1E2ABA18B123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75E8802A-DA55-417F-AEFE-094682266A06}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -254,27 +254,12 @@
     <t>None</t>
   </si>
   <si>
-    <t>("DUNE", "Frank Herbert", Genre.FICTION)</t>
-  </si>
-  <si>
-    <t>("", "Frank Herbert", Genre.FICTION)</t>
-  </si>
-  <si>
-    <t>("DUNE", "", Genre.FICTION)</t>
-  </si>
-  <si>
-    <t>("DUNE", "Frank Herbert", "INVALID)</t>
-  </si>
-  <si>
     <t>Pass/No errors</t>
   </si>
   <si>
     <t>Raise ValueError</t>
   </si>
   <si>
-    <t>LibraryItem("DUNE", "Frank Herbert", Genre.FICTION)</t>
-  </si>
-  <si>
     <t>Returns title</t>
   </si>
   <si>
@@ -285,6 +270,54 @@
   </si>
   <si>
     <t>Philip Pacla-on</t>
+  </si>
+  <si>
+    <t>Exception raised when invalid item id</t>
+  </si>
+  <si>
+    <t>exception raised when invalid is borrowed</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>returns item_id attribute</t>
+  </si>
+  <si>
+    <t>return is_borrowed attribute</t>
+  </si>
+  <si>
+    <t>is_ borrowed</t>
+  </si>
+  <si>
+    <t>("INVALID ID", "DUNE",  "Frank Herbert", "INVALID", False)</t>
+  </si>
+  <si>
+    <t>(1, "DUNE",  "Frank Herbert", "INVALID", "Not a boolean")</t>
+  </si>
+  <si>
+    <t>Raises ValueError</t>
+  </si>
+  <si>
+    <t>(1, "DUNE", "Frank Herbert", Genre.FICTION, False)</t>
+  </si>
+  <si>
+    <t>(1, "", "Frank Herbert", Genre.FICTION, False)</t>
+  </si>
+  <si>
+    <t>(1, "DUNE", "", Genre.FICTION, False)</t>
+  </si>
+  <si>
+    <t>(1, "DUNE", "Frank Herbert", "INVALID, False)</t>
+  </si>
+  <si>
+    <t>LibraryItem(1, "DUNE", "Frank Herbert", Genre.FICTION, False)</t>
+  </si>
+  <si>
+    <t>Returns item_Id</t>
+  </si>
+  <si>
+    <t>returns is_borrowed</t>
   </si>
 </sst>
 </file>
@@ -746,6 +779,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1145,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1214,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D3" s="16"/>
     </row>
@@ -1228,10 +1265,10 @@
         <v>22</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,10 +1286,10 @@
         <v>22</v>
       </c>
       <c r="F8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1270,10 +1307,10 @@
         <v>22</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1291,10 +1328,10 @@
         <v>22</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,13 +1345,13 @@
         <v>17</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1328,13 +1365,13 @@
         <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1348,54 +1385,94 @@
         <v>19</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12">
         <v>11</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="12">
         <v>12</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>13</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="12">

</xml_diff>